<commit_message>
parallel: <<lab2>>: update code and expiriment results
</commit_message>
<xml_diff>
--- a/Parallel and distributed systems/parallel/lab2/results_lab2_1.xlsx
+++ b/Parallel and distributed systems/parallel/lab2/results_lab2_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t xml:space="preserve">Номер задачи</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t xml:space="preserve">1_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consecutive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">continuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cyclic</t>
   </si>
   <si>
     <t xml:space="preserve">P=1</t>
@@ -82,7 +94,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -120,6 +132,29 @@
       <family val="0"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FFA31515"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9.5"/>
+      <color rgb="FFA31515"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,7 +205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -203,6 +238,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -213,6 +260,14 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -224,6 +279,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFA31515"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -232,16 +347,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:L30"/>
+  <dimension ref="A2:L45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -447,25 +562,174 @@
         <v>0.462476505297305</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <f aca="false">AVERAGE(B33:B35)</f>
+        <v>671.265666666667</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <f aca="false">AVERAGE(B38:B40)</f>
+        <v>673.319333333333</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <f aca="false">AVERAGE(C38:C40)</f>
+        <v>335.860333333333</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <f aca="false">C8/D8</f>
+        <v>2.00475991508375</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <f aca="false">E8/2</f>
+        <v>1.00237995754188</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <f aca="false">AVERAGE(D38:D40)</f>
+        <v>231.430333333333</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <f aca="false">C8/G8</f>
+        <v>2.90938237713005</v>
+      </c>
+      <c r="I8" s="6" t="n">
+        <f aca="false">H8/3</f>
+        <v>0.969794125710017</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <f aca="false">AVERAGE(E38:E40)</f>
+        <v>182.36</v>
+      </c>
+      <c r="K8" s="6" t="n">
+        <f aca="false">C8/J8</f>
+        <v>3.69225341814725</v>
+      </c>
+      <c r="L8" s="6" t="n">
+        <f aca="false">K8/4</f>
+        <v>0.923063354536814</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <f aca="false">AVERAGE(B43:B45)</f>
+        <v>668.641</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <f aca="false">AVERAGE(C43:C45)</f>
+        <v>421.707666666667</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <f aca="false">C9/D9</f>
+        <v>1.58555571276469</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <f aca="false">E9/2</f>
+        <v>0.792777856382344</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <f aca="false">AVERAGE(D43:D45)</f>
+        <v>244.378666666667</v>
+      </c>
+      <c r="H9" s="6" t="n">
+        <f aca="false">C9/G9</f>
+        <v>2.73608580127016</v>
+      </c>
+      <c r="I9" s="6" t="n">
+        <f aca="false">H9/3</f>
+        <v>0.912028600423387</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <f aca="false">AVERAGE(E43:E45)</f>
+        <v>201.572</v>
+      </c>
+      <c r="K9" s="6" t="n">
+        <f aca="false">C9/J9</f>
+        <v>3.3171323398091</v>
+      </c>
+      <c r="L9" s="6" t="n">
+        <f aca="false">K9/4</f>
+        <v>0.829283084952275</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>15</v>
+      <c r="B17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="9" t="n">
+      <c r="B18" s="12" t="n">
         <v>13.967137</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -479,7 +743,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="9" t="n">
+      <c r="B19" s="12" t="n">
         <v>15.085691</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -493,7 +757,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="10" t="n">
+      <c r="B20" s="13" t="n">
         <v>12.084065</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -510,17 +774,17 @@
       <c r="A22" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>15</v>
+      <c r="B22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -569,17 +833,17 @@
       <c r="A27" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>15</v>
+      <c r="B27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,6 +886,147 @@
       </c>
       <c r="E30" s="0" t="n">
         <v>4.334059</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="n">
+        <v>671.785</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="n">
+        <v>671.654</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="n">
+        <v>670.358</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="n">
+        <v>676.394</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>335.388</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>232.91</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>178.773</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="n">
+        <v>676.065</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>336.928</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>233.504</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>185.499</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="n">
+        <v>667.499</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>335.265</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>227.877</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>182.808</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="n">
+        <v>666.946</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>353.781</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>234.99</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>192.441</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="n">
+        <v>668.95</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>485.699</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>249.865</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>189.713</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="n">
+        <v>670.027</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>425.643</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>248.281</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>222.562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
parallel: <<lab2>>: update file
</commit_message>
<xml_diff>
--- a/Parallel and distributed systems/parallel/lab2/results_lab2_1.xlsx
+++ b/Parallel and distributed systems/parallel/lab2/results_lab2_1.xlsx
@@ -94,7 +94,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -128,21 +128,6 @@
     <font>
       <sz val="9.5"/>
       <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="0"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="9.5"/>
-      <color rgb="FFA31515"/>
-      <name val="Consolas"/>
-      <family val="0"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9.5"/>
-      <color rgb="FFA31515"/>
       <name val="Consolas"/>
       <family val="0"/>
       <charset val="204"/>
@@ -205,7 +190,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,18 +223,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,7 +247,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -279,66 +260,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFA31515"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -349,8 +270,8 @@
   </sheetPr>
   <dimension ref="A2:L45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -563,7 +484,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="6" t="n">
@@ -573,36 +494,36 @@
         <f aca="false">AVERAGE(B33:B35)</f>
         <v>671.265666666667</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="6" t="n">
@@ -650,7 +571,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="6" t="n">
@@ -715,21 +636,21 @@
       <c r="A17" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12" t="n">
+      <c r="B18" s="11" t="n">
         <v>13.967137</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -743,7 +664,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="12" t="n">
+      <c r="B19" s="11" t="n">
         <v>15.085691</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -757,7 +678,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="13" t="n">
+      <c r="B20" s="12" t="n">
         <v>12.084065</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -774,16 +695,16 @@
       <c r="A22" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -833,16 +754,16 @@
       <c r="A27" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -889,10 +810,10 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -912,19 +833,19 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -971,19 +892,19 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="10" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove and update rtesults
</commit_message>
<xml_diff>
--- a/Parallel and distributed systems/parallel/lab2/results_lab2_1.xlsx
+++ b/Parallel and distributed systems/parallel/lab2/results_lab2_1.xlsx
@@ -199,7 +199,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -232,6 +232,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,8 +244,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -344,7 +348,7 @@
   <dimension ref="A2:O45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -607,7 +611,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="6" t="n">
@@ -617,45 +621,45 @@
         <f aca="false">AVERAGE(B33:B35)</f>
         <v>671.265666666667</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="N7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="O7" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="6" t="n">
@@ -715,7 +719,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="6" t="n">
@@ -792,19 +796,19 @@
       <c r="O10" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G17" s="0" t="s">
@@ -812,8 +816,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11"/>
-      <c r="B18" s="13" t="n">
+      <c r="A18" s="12"/>
+      <c r="B18" s="14" t="n">
         <v>13.967137</v>
       </c>
       <c r="C18" s="6" t="n">
@@ -830,8 +834,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
-      <c r="B19" s="13" t="n">
+      <c r="A19" s="12"/>
+      <c r="B19" s="14" t="n">
         <v>15.085691</v>
       </c>
       <c r="C19" s="6" t="n">
@@ -848,8 +852,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11"/>
-      <c r="B20" s="13" t="n">
+      <c r="A20" s="12"/>
+      <c r="B20" s="14" t="n">
         <v>12.084065</v>
       </c>
       <c r="C20" s="6" t="n">
@@ -866,24 +870,24 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="6" t="n">
         <v>8.077931</v>
       </c>
@@ -898,7 +902,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="6" t="n">
         <v>11.305724</v>
       </c>
@@ -913,7 +917,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="6" t="n">
         <v>10.934025</v>
       </c>
@@ -937,16 +941,16 @@
       <c r="A27" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="13" t="s">
         <v>20</v>
       </c>
     </row>
@@ -993,10 +997,10 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="15"/>
+      <c r="B32" s="16"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="n">
@@ -1014,19 +1018,19 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="13" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1073,19 +1077,19 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="13" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>